<commit_message>
Revision hasta TIPO DE PERSONA TITULAR, quedaron columnas por corregir
</commit_message>
<xml_diff>
--- a/ID_con_problemas_vacios.xlsx
+++ b/ID_con_problemas_vacios.xlsx
@@ -469,7 +469,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 1</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 2</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 3</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 4</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 5</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 6</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 7</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 8</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 9</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 10</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 11</t>
         </is>
       </c>
     </row>
@@ -612,7 +612,7 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 12</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 13</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 14</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 15</t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 16</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 17</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 18</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 19</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 20</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 21</t>
         </is>
       </c>
     </row>
@@ -742,7 +742,7 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>SIN REGISTRO</t>
+          <t>SIN REGISTRO 22</t>
         </is>
       </c>
     </row>

</xml_diff>